<commit_message>
Updated FormatConversion.xlsx with -3 inches formulas.
</commit_message>
<xml_diff>
--- a/FormatConversion.xlsx
+++ b/FormatConversion.xlsx
@@ -10,26 +10,35 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BridgeDBValue">Sheet1!$A$2</definedName>
+    <definedName name="BridgeDBValue">Sheet1!$B$2</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Feet</t>
   </si>
   <si>
     <t>Inches</t>
   </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Reported</t>
+  </si>
+  <si>
+    <t>From DB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -37,16 +46,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -54,14 +76,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -361,36 +401,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>1505</v>
       </c>
-      <c r="B2">
+      <c r="C2" s="1">
         <f>ROUND(BridgeDBValue/100,0)*12+MOD(BridgeDBValue,100)</f>
         <v>185</v>
       </c>
-      <c r="C2">
+      <c r="D2" s="1">
         <f>ROUND(BridgeDBValue/100,0)+(MOD(BridgeDBValue,100)/12)</f>
         <v>15.416666666666666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <f>(ROUND(BridgeDBValue/100,0)*12+MOD(BridgeDBValue,100))-3</f>
+        <v>182</v>
+      </c>
+      <c r="D3" s="1">
+        <f>(ROUND(BridgeDBValue/100,0)+(MOD(BridgeDBValue,100)/12))-3/12</f>
+        <v>15.166666666666666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1400</v>
+      </c>
+      <c r="C5" s="1">
+        <f>ROUND(B5/100,0)*12+MOD(BridgeDBValue,100)</f>
+        <v>173</v>
+      </c>
+      <c r="D5" s="1">
+        <f>ROUND(B5/100,0)+(MOD(B5,100)/12)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <f>(ROUND(B5/100,0)*12+MOD(B5,100))-3</f>
+        <v>165</v>
+      </c>
+      <c r="D6" s="1">
+        <f>(ROUND(B5/100,0)+(MOD(B5,100)/12))-3/12</f>
+        <v>13.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>